<commit_message>
Completed tasks in Codechanges.xslx
Completed some of the simple tasks in CodeChanges.xlsx except adding the try catch block
</commit_message>
<xml_diff>
--- a/CodeChanges.xlsx
+++ b/CodeChanges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sanketh\Github\CsvToVcf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daryl\Documents\GitHub\CsvToVcf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BF0558-6FD0-4E8C-A75E-9FF8730797F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E39CA-3D4C-4138-A436-2640A38E8F17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. 7 Jan 2020" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Sl. No</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Implement bootstrap 4 for your layouts, and form controls</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Fuck you</t>
   </si>
 </sst>
 </file>
@@ -126,10 +132,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,33 +420,33 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -448,119 +454,137 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>54</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>57</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>79</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -568,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -576,7 +600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -584,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -600,5 +624,6 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made most of the changes
Made most of the changes requested except some which I have no idea how to do!
</commit_message>
<xml_diff>
--- a/CodeChanges.xlsx
+++ b/CodeChanges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sanketh\Github\CsvToVcf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Visual Studio 2019\Trial\Sample\CsvToVcf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EAE216-EB8D-41F5-B732-5F6910991675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF3F018-C7BF-48A7-A113-7988B4F4E4AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. 7 Jan 2020" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Sl. No</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Delete all csv files once it has been successfully dowloaded</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Kinda</t>
+  </si>
+  <si>
+    <t>Nope</t>
   </si>
 </sst>
 </file>
@@ -485,15 +494,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -516,7 +525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -533,7 +542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -550,7 +559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -567,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -584,7 +593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -601,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -618,7 +627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -635,7 +644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -652,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -663,7 +672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -674,7 +683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -685,7 +694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -711,18 +720,18 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -737,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -748,10 +757,13 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
@@ -762,10 +774,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
       <c r="C4" t="s">
         <v>32</v>
       </c>
@@ -776,9 +791,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -788,10 +806,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
@@ -802,10 +823,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" t="s">
         <v>32</v>
       </c>
@@ -813,9 +837,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
@@ -824,32 +851,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="C3:E6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:E6">
     <sortCondition ref="C3"/>
   </sortState>
   <mergeCells count="1">

</xml_diff>